<commit_message>
finally fix even better
</commit_message>
<xml_diff>
--- a/excel/spotify-2000-clean.xlsx
+++ b/excel/spotify-2000-clean.xlsx
@@ -70,7 +70,7 @@
     <t>The Pretender</t>
   </si>
   <si>
-    <t>Waitin On A Sunny Day</t>
+    <t>Waitin' On A Sunny Day</t>
   </si>
   <si>
     <t>The Road Ahead (Miles Of The Unknown)</t>
@@ -94,7 +94,7 @@
     <t>Seven Nation Army</t>
   </si>
   <si>
-    <t>Im going home</t>
+    <t>I'm going home</t>
   </si>
   <si>
     <t>Fluorescent Adolescent</t>
@@ -124,7 +124,7 @@
     <t>Smokers Outside the Hospital Doors</t>
   </si>
   <si>
-    <t>Cleanin Out My Closet</t>
+    <t>Cleanin' Out My Closet</t>
   </si>
   <si>
     <t>Der Weg</t>
@@ -139,7 +139,7 @@
     <t>Chasing Pavements</t>
   </si>
   <si>
-    <t>Dont Know Why</t>
+    <t>Don't Know Why</t>
   </si>
   <si>
     <t>Tears Dry On Their Own</t>
@@ -160,7 +160,7 @@
     <t>De Weg</t>
   </si>
   <si>
-    <t>Dont Let Me Be Misunderstood</t>
+    <t>Don't Let Me Be Misunderstood</t>
   </si>
   <si>
     <t>Traffic - Radio Edit</t>
@@ -184,7 +184,7 @@
     <t>Run</t>
   </si>
   <si>
-    <t>Youre The First, The Last, My Everything</t>
+    <t>You're The First, The Last, My Everything</t>
   </si>
   <si>
     <t>The Day After Tomorrow</t>
@@ -205,7 +205,7 @@
     <t>Grounds for Divorce</t>
   </si>
   <si>
-    <t>Sometimes You Cant Make It On Your Own</t>
+    <t>Sometimes You Can't Make It On Your Own</t>
   </si>
   <si>
     <t>Listen (From the Motion Picture Dreamgirls)</t>
@@ -256,7 +256,7 @@
     <t>Dirty Diana</t>
   </si>
   <si>
-    <t>Sad Mans Tongue</t>
+    <t>Sad Man's Tongue</t>
   </si>
   <si>
     <t>One Day Like This</t>
@@ -280,7 +280,7 @@
     <t>Times Like These</t>
   </si>
   <si>
-    <t>Im Gonna Be (500 Miles)</t>
+    <t>I'm Gonna Be (500 Miles)</t>
   </si>
   <si>
     <t>Blauwe Ruis</t>
@@ -319,7 +319,7 @@
     <t>Forever Autumn</t>
   </si>
   <si>
-    <t>Everybodys Changing</t>
+    <t>Everybody's Changing</t>
   </si>
   <si>
     <t>How to Save a Life</t>
@@ -331,7 +331,7 @@
     <t>Lose Yourself - From 8 Mile Soundtrack</t>
   </si>
   <si>
-    <t>Europa (Earths Cry Heavens Smile)</t>
+    <t>Europa (Earth's Cry Heaven's Smile)</t>
   </si>
   <si>
     <t>Feeling Good</t>
@@ -349,7 +349,7 @@
     <t>Single Ladies (Put a Ring on It)</t>
   </si>
   <si>
-    <t>Youre the Voice</t>
+    <t>You're the Voice</t>
   </si>
   <si>
     <t>Voltooid Verleden Tijd</t>
@@ -379,7 +379,7 @@
     <t>Tribute</t>
   </si>
   <si>
-    <t>You Know Im No Good</t>
+    <t>You Know I'm No Good</t>
   </si>
   <si>
     <t>Love Is A Battlefield</t>
@@ -424,7 +424,7 @@
     <t>Going To A Town</t>
   </si>
   <si>
-    <t>A Gentlemans Excuse Me</t>
+    <t>A Gentleman's Excuse Me</t>
   </si>
   <si>
     <t>Sailing to Philadelphia</t>
@@ -433,7 +433,7 @@
     <t>Accidentally In Love</t>
   </si>
   <si>
-    <t>Its Raining Men</t>
+    <t>It's Raining Men</t>
   </si>
   <si>
     <t>Goodnight Saigon</t>
@@ -451,10 +451,10 @@
     <t>Everything</t>
   </si>
   <si>
-    <t>Comptine dun autre été, laprès-midi</t>
-  </si>
-  <si>
-    <t>The Man Who Cant Be Moved</t>
+    <t>Comptine d'un autre été, l'après-midi</t>
+  </si>
+  <si>
+    <t>The Man Who Can't Be Moved</t>
   </si>
   <si>
     <t>Halo</t>
@@ -478,10 +478,10 @@
     <t>Father &amp; Friend</t>
   </si>
   <si>
-    <t>(Ive Had) The Time of My Life - From Dirty Dancing Soundtrack</t>
-  </si>
-  <si>
-    <t>The Blowers Daughter</t>
+    <t>(I've Had) The Time of My Life - From Dirty Dancing Soundtrack</t>
+  </si>
+  <si>
+    <t>The Blower's Daughter</t>
   </si>
   <si>
     <t>Magnificent</t>
@@ -508,7 +508,7 @@
     <t>The Real Slim Shady</t>
   </si>
   <si>
-    <t>Stuck In A Moment You Cant Get Out Of</t>
+    <t>Stuck In A Moment You Can't Get Out Of</t>
   </si>
   <si>
     <t>Starlight</t>
@@ -520,19 +520,19 @@
     <t>Time To Say Goodbye (Con Te Partirò)</t>
   </si>
   <si>
-    <t>Silence (feat. Sarah McLachlan) - DJ Tiëstos In Search of Sunrise Edit</t>
+    <t>Silence (feat. Sarah McLachlan) - DJ Tiësto's In Search of Sunrise Edit</t>
   </si>
   <si>
     <t>Supermassive Black Hole</t>
   </si>
   <si>
-    <t>Pak Maar Mn Hand</t>
+    <t>Pak Maar M'n Hand</t>
   </si>
   <si>
     <t>Bombay</t>
   </si>
   <si>
-    <t>Mary Janes Last Dance</t>
+    <t>Mary Jane's Last Dance</t>
   </si>
   <si>
     <t>Oerend Hard</t>
@@ -547,7 +547,7 @@
     <t>Wake Me up When September Ends</t>
   </si>
   <si>
-    <t>Cant Stop</t>
+    <t>Can't Stop</t>
   </si>
   <si>
     <t>Driving Home for Christmas</t>
@@ -739,7 +739,7 @@
     <t>Like a Prayer</t>
   </si>
   <si>
-    <t>Rockin All Over The World</t>
+    <t>Rockin' All Over The World</t>
   </si>
   <si>
     <t>Dear Mr. President</t>
@@ -805,7 +805,7 @@
     <t>Bird of Paradise</t>
   </si>
   <si>
-    <t>Im Yours</t>
+    <t>I'm Yours</t>
   </si>
   <si>
     <t>Onderweg</t>
@@ -844,7 +844,7 @@
     <t>Nine Million Bicycles</t>
   </si>
   <si>
-    <t>Its My Life</t>
+    <t>It's My Life</t>
   </si>
   <si>
     <t>Mooie Dag</t>
@@ -925,7 +925,7 @@
     <t>One More Time</t>
   </si>
   <si>
-    <t>(Youre The) Devil in Disguise</t>
+    <t>(You're The) Devil in Disguise</t>
   </si>
   <si>
     <t>TRUE - Single Edit</t>
@@ -955,7 +955,7 @@
     <t>Nutbush City Limits</t>
   </si>
   <si>
-    <t>Do They Know Its Christmas? - 1984 Version</t>
+    <t>Do They Know It's Christmas? - 1984 Version</t>
   </si>
   <si>
     <t>Changes</t>
@@ -1072,10 +1072,10 @@
     <t>Turning Tables</t>
   </si>
   <si>
-    <t>Luv U More - K&amp;As Radio blast</t>
-  </si>
-  <si>
-    <t>Drivers Seat</t>
+    <t>Luv U More - K&amp;A's Radio blast</t>
+  </si>
+  <si>
+    <t>Driver's Seat</t>
   </si>
   <si>
     <t>Zing Voor Me</t>
@@ -1099,7 +1099,7 @@
     <t>Run the World (Girls)</t>
   </si>
   <si>
-    <t>I Won T Let You Down</t>
+    <t>I Won' T Let You Down</t>
   </si>
   <si>
     <t>Love On Top</t>
@@ -1126,7 +1126,7 @@
     <t>Georgia on My Mind</t>
   </si>
   <si>
-    <t>Ive Just Lost Somebody</t>
+    <t>I've Just Lost Somebody</t>
   </si>
   <si>
     <t>Skyfall - Full Length</t>
@@ -1180,7 +1180,7 @@
     <t>Sovereign Light Café</t>
   </si>
   <si>
-    <t>Cant Hold Us - feat. Ray Dalton</t>
+    <t>Can't Hold Us - feat. Ray Dalton</t>
   </si>
   <si>
     <t>Lover of the Light</t>
@@ -1204,7 +1204,7 @@
     <t>When I Was Your Man</t>
   </si>
   <si>
-    <t>I Wont Give Up</t>
+    <t>I Won't Give Up</t>
   </si>
   <si>
     <t>Slapeloze Nachten</t>
@@ -1237,7 +1237,7 @@
     <t>Diamonds</t>
   </si>
   <si>
-    <t>Its Time</t>
+    <t>It's Time</t>
   </si>
   <si>
     <t>Little Talks</t>
@@ -1327,7 +1327,7 @@
     <t>I Sat By The Ocean</t>
   </si>
   <si>
-    <t>Everybody (Backstreets Back) - Radio Edit</t>
+    <t>Everybody (Backstreet's Back) - Radio Edit</t>
   </si>
   <si>
     <t>A Ton of Love</t>
@@ -1384,7 +1384,7 @@
     <t>Red Eyes</t>
   </si>
   <si>
-    <t>Lamour Toujours (Small Mix)</t>
+    <t>L'amour Toujours (Small Mix)</t>
   </si>
   <si>
     <t>See Me, Feel Me - Single Version</t>
@@ -1534,7 +1534,7 @@
     <t>Do I Ever</t>
   </si>
   <si>
-    <t>CANT STOP THE FEELING! (Original Song from DreamWorks Animations TROLLS)</t>
+    <t>CAN'T STOP THE FEELING! (Original Song from DreamWorks Animation's TROLLS)</t>
   </si>
   <si>
     <t>Whatever You Want</t>
@@ -1555,7 +1555,7 @@
     <t>Bridges</t>
   </si>
   <si>
-    <t>I Just Cant Help Believin</t>
+    <t>I Just Can't Help Believin'</t>
   </si>
   <si>
     <t>Love &amp; Hate</t>
@@ -1642,7 +1642,7 @@
     <t>Through the Barricades - Remastered</t>
   </si>
   <si>
-    <t>Freedom! 90 - Remastered</t>
+    <t>Freedom! '90 - Remastered</t>
   </si>
   <si>
     <t>Amsterdam</t>
@@ -1675,7 +1675,7 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Rappers Delight</t>
+    <t>Rapper's Delight</t>
   </si>
   <si>
     <t>Pain</t>
@@ -1786,7 +1786,7 @@
     <t>Always Remember Us This Way</t>
   </si>
   <si>
-    <t>Why Dont You Do Right</t>
+    <t>Why Don't You Do Right</t>
   </si>
   <si>
     <t>De Zon Op</t>
@@ -1825,7 +1825,7 @@
     <t>A Whiter Shade of Pale - Original Single Version</t>
   </si>
   <si>
-    <t>Dont You (Forget About Me)</t>
+    <t>Don't You (Forget About Me)</t>
   </si>
   <si>
     <t>The Load-Out - Remastered</t>
@@ -1906,7 +1906,7 @@
     <t>Immigrant Song - Remaster</t>
   </si>
   <si>
-    <t>Wholl Stop The Rain</t>
+    <t>Who'll Stop The Rain</t>
   </si>
   <si>
     <t>Our House</t>
@@ -1930,7 +1930,7 @@
     <t>I Heard It Through The Grapevine</t>
   </si>
   <si>
-    <t>Since Ive Been Loving You - 1990 Remaster</t>
+    <t>Since I've Been Loving You - 1990 Remaster</t>
   </si>
   <si>
     <t>The Man Who Sold the World - 2015 Remaster</t>
@@ -1951,7 +1951,7 @@
     <t>Fire and Rain</t>
   </si>
   <si>
-    <t>Lookin Out My Back Door</t>
+    <t>Lookin' Out My Back Door</t>
   </si>
   <si>
     <t>25 or 6 to 4 - 2002 Remaster</t>
@@ -2002,7 +2002,7 @@
     <t>Me and Bobby McGee</t>
   </si>
   <si>
-    <t>Baba ORiley</t>
+    <t>Baba O'Riley</t>
   </si>
   <si>
     <t>Life on Mars? - 2015 Remaster</t>
@@ -2011,7 +2011,7 @@
     <t>I Am...I Said - Single Version</t>
   </si>
   <si>
-    <t>Aint No Sunshine</t>
+    <t>Ain't No Sunshine</t>
   </si>
   <si>
     <t>Wild Horses</t>
@@ -2020,7 +2020,7 @@
     <t>L.A. Woman</t>
   </si>
   <si>
-    <t>Whats Going On</t>
+    <t>What's Going On</t>
   </si>
   <si>
     <t>Halo of Flies</t>
@@ -2047,7 +2047,7 @@
     <t>Brown Sugar - Remastered</t>
   </si>
   <si>
-    <t>Youve Got a Friend</t>
+    <t>You've Got a Friend</t>
   </si>
   <si>
     <t>Locomotive Breath</t>
@@ -2077,7 +2077,7 @@
     <t>Maggie May</t>
   </si>
   <si>
-    <t>Wont Get Fooled Again - Original Album Version</t>
+    <t>Won't Get Fooled Again - Original Album Version</t>
   </si>
   <si>
     <t>After Midnight</t>
@@ -2113,7 +2113,7 @@
     <t>Perfect Day</t>
   </si>
   <si>
-    <t>Rocket Man (I Think Its Going To Be A Long, Long Time)</t>
+    <t>Rocket Man (I Think It's Going To Be A Long, Long Time)</t>
   </si>
   <si>
     <t>Heart of Gold - 2009 Remaster</t>
@@ -2134,7 +2134,7 @@
     <t>Lola - Live</t>
   </si>
   <si>
-    <t>Easy Livin</t>
+    <t>Easy Livin'</t>
   </si>
   <si>
     <t>Ben - Single Version</t>
@@ -2143,10 +2143,10 @@
     <t>Walk On the Wild Side</t>
   </si>
   <si>
-    <t>Shes A Rainbow - Full Version / With Intro</t>
-  </si>
-  <si>
-    <t>Youre so Vain</t>
+    <t>She's A Rainbow - Full Version / With Intro</t>
+  </si>
+  <si>
+    <t>You're so Vain</t>
   </si>
   <si>
     <t>Ziggy Stardust - 2012 Remaster</t>
@@ -2161,7 +2161,7 @@
     <t>Top Of The World</t>
   </si>
   <si>
-    <t>Schools Out</t>
+    <t>School's Out</t>
   </si>
   <si>
     <t>A Thing Called Love</t>
@@ -2170,7 +2170,7 @@
     <t>Harvest - 2009 Remaster</t>
   </si>
   <si>
-    <t>Sylvias Mother</t>
+    <t>Sylvia's Mother</t>
   </si>
   <si>
     <t>Close to the Edge (i. The Solid Time of Change, ii. Total Mass Retain, iii. I Get up I Get Down, iv. Seasons of Man) - 2003 Remaster</t>
@@ -2242,7 +2242,7 @@
     <t>Tequila Sunrise - 2013 Remaster</t>
   </si>
   <si>
-    <t>Knockin On Heavens Door - Remastered</t>
+    <t>Knockin' On Heaven's Door - Remastered</t>
   </si>
   <si>
     <t>Burning Love</t>
@@ -2260,10 +2260,10 @@
     <t>The Joker</t>
   </si>
   <si>
-    <t>Long Train Runnin</t>
-  </si>
-  <si>
-    <t>Ill Have To Say I Love You In A Song</t>
+    <t>Long Train Runnin'</t>
+  </si>
+  <si>
+    <t>I'll Have To Say I Love You In A Song</t>
   </si>
   <si>
     <t>The Jean Genie - 2013 Remaster</t>
@@ -2275,7 +2275,7 @@
     <t>Woman from Tokyo</t>
   </si>
   <si>
-    <t>Lets Get It On</t>
+    <t>Let's Get It On</t>
   </si>
   <si>
     <t>School</t>
@@ -2293,7 +2293,7 @@
     <t>Waterloo</t>
   </si>
   <si>
-    <t>Annies Song</t>
+    <t>Annie's Song</t>
   </si>
   <si>
     <t>Dreamer</t>
@@ -2317,7 +2317,7 @@
     <t>I Will Always Love You</t>
   </si>
   <si>
-    <t>Thank God Im a Country Boy</t>
+    <t>Thank God I'm a Country Boy</t>
   </si>
   <si>
     <t>The Air That I Breathe - 2008 Remaster</t>
@@ -2335,13 +2335,13 @@
     <t>Fox On The Run</t>
   </si>
   <si>
-    <t>You Aint Seen Nothing Yet</t>
+    <t>You Ain't Seen Nothing Yet</t>
   </si>
   <si>
     <t>Mandy</t>
   </si>
   <si>
-    <t>Cant Get It out of My Head</t>
+    <t>Can't Get It out of My Head</t>
   </si>
   <si>
     <t>The Way We Were</t>
@@ -2377,16 +2377,16 @@
     <t>Thunder Road</t>
   </si>
   <si>
-    <t>Im Not In Love</t>
+    <t>I'm Not In Love</t>
   </si>
   <si>
     <t>Rhiannon</t>
   </si>
   <si>
-    <t>Lyin Eyes - 2013 Remaster</t>
-  </si>
-  <si>
-    <t>Youre My Best Friend - Remastered 2011</t>
+    <t>Lyin' Eyes - 2013 Remaster</t>
+  </si>
+  <si>
+    <t>You're My Best Friend - Remastered 2011</t>
   </si>
   <si>
     <t>Jungleland</t>
@@ -2410,7 +2410,7 @@
     <t>50 Ways to Leave Your Lover</t>
   </si>
   <si>
-    <t>Its A Long Way There - 2010 Digital Remaster</t>
+    <t>It's A Long Way There - 2010 Digital Remaster</t>
   </si>
   <si>
     <t>Crazy On You</t>
@@ -2467,7 +2467,7 @@
     <t>More Than a Feeling</t>
   </si>
   <si>
-    <t>(Dont Fear) The Reaper</t>
+    <t>(Don't Fear) The Reaper</t>
   </si>
   <si>
     <t>New Kid in Town - 2013 Remaster</t>
@@ -2500,19 +2500,19 @@
     <t>Golden Years - 2016 Remaster</t>
   </si>
   <si>
-    <t>Isnt She Lovely</t>
+    <t>Isn't She Lovely</t>
   </si>
   <si>
     <t>I Wish</t>
   </si>
   <si>
-    <t>Tom Trauberts Blues (Four Sheets To The Wind In Copenhagen)</t>
+    <t>Tom Traubert's Blues (Four Sheets To The Wind In Copenhagen)</t>
   </si>
   <si>
     <t>The Boys Are Back In Town</t>
   </si>
   <si>
-    <t>Livin Thing</t>
+    <t>Livin' Thing</t>
   </si>
   <si>
     <t>Sir Duke</t>
@@ -2539,7 +2539,7 @@
     <t>Wasted Time - 2013 Remaster</t>
   </si>
   <si>
-    <t>Theme From Mahogany (Do You Know Where Youre Going To) - Single Version</t>
+    <t>Theme From Mahogany (Do You Know Where You're Going To) - Single Version</t>
   </si>
   <si>
     <t>Heroes - 2017 Remaster</t>
@@ -2554,7 +2554,7 @@
     <t>Mr. Blue Sky</t>
   </si>
   <si>
-    <t>Fools Overture</t>
+    <t>Fool's Overture</t>
   </si>
   <si>
     <t>Whole Lotta Rosie</t>
@@ -2572,7 +2572,7 @@
     <t>We Are The Champions - Remastered 2011</t>
   </si>
   <si>
-    <t>Shes Always a Woman</t>
+    <t>She's Always a Woman</t>
   </si>
   <si>
     <t>Worn Down Piano</t>
@@ -2596,10 +2596,10 @@
     <t>Lust For Life</t>
   </si>
   <si>
-    <t>Shes Not There</t>
-  </si>
-  <si>
-    <t>Stayin Alive</t>
+    <t>She's Not There</t>
+  </si>
+  <si>
+    <t>Stayin' Alive</t>
   </si>
   <si>
     <t>Psycho Killer - 2005 Remaster</t>
@@ -2614,7 +2614,7 @@
     <t>Let There Be Rock</t>
   </si>
   <si>
-    <t>Dont Stop - 2004 Remaster</t>
+    <t>Don't Stop - 2004 Remaster</t>
   </si>
   <si>
     <t>I Feel Love</t>
@@ -2641,7 +2641,7 @@
     <t>You Took The Words Right Out of My Mouth (Hot Summer Night)</t>
   </si>
   <si>
-    <t>Two Out of Three Aint Bad</t>
+    <t>Two Out of Three Ain't Bad</t>
   </si>
   <si>
     <t>Barracuda</t>
@@ -2680,7 +2680,7 @@
     <t>Lovely Day</t>
   </si>
   <si>
-    <t>Isnt It Time</t>
+    <t>Isn't It Time</t>
   </si>
   <si>
     <t>Anarchy in the U.K.</t>
@@ -2692,7 +2692,7 @@
     <t>Sultans of Swing</t>
   </si>
   <si>
-    <t>Dont Stop Me Now - 2011 Mix</t>
+    <t>Don't Stop Me Now - 2011 Mix</t>
   </si>
   <si>
     <t>Wuthering Heights</t>
@@ -2719,7 +2719,7 @@
     <t>Fat Bottomed Girls - Single Version</t>
   </si>
   <si>
-    <t>Runnin with the Devil - 2015 Remaster</t>
+    <t>Runnin' with the Devil - 2015 Remaster</t>
   </si>
   <si>
     <t>Bicycle Race - Remastered 2011</t>
@@ -2752,7 +2752,7 @@
     <t>Rivers of Babylon</t>
   </si>
   <si>
-    <t>Dont Look Back</t>
+    <t>Don't Look Back</t>
   </si>
   <si>
     <t>Beast Of Burden - Remastered</t>
@@ -2767,7 +2767,7 @@
     <t>Fire</t>
   </si>
   <si>
-    <t>You Dont Bring Me Flowers</t>
+    <t>You Don't Bring Me Flowers</t>
   </si>
   <si>
     <t>Water of Love</t>
@@ -2788,7 +2788,7 @@
     <t>The Logical Song - Remastered 2010</t>
   </si>
   <si>
-    <t>I Was Made For Lovin You</t>
+    <t>I Was Made For Lovin' You</t>
   </si>
   <si>
     <t>Gimme! Gimme! Gimme! (A Man After Midnight)</t>
@@ -2827,7 +2827,7 @@
     <t>Boogie Wonderland</t>
   </si>
   <si>
-    <t>Boys Dont Cry - Single Version</t>
+    <t>Boys Don't Cry - Single Version</t>
   </si>
   <si>
     <t>Voulez-Vous</t>
@@ -2839,7 +2839,7 @@
     <t>MacArthur Park - Single Version</t>
   </si>
   <si>
-    <t>Dont Stop Til You Get Enough - Single Version</t>
+    <t>Don't Stop 'Til You Get Enough - Single Version</t>
   </si>
   <si>
     <t>London Calling - Remastered</t>
@@ -2854,7 +2854,7 @@
     <t>Walking On The Moon</t>
   </si>
   <si>
-    <t>Dont Bring Me Down</t>
+    <t>Don't Bring Me Down</t>
   </si>
   <si>
     <t>Tragedy</t>
@@ -2884,7 +2884,7 @@
     <t>Weekend</t>
   </si>
   <si>
-    <t>Dancin Fool</t>
+    <t>Dancin' Fool</t>
   </si>
   <si>
     <t>We Belong to the Night</t>
@@ -2995,16 +2995,16 @@
     <t>Enola Gay - Remastered</t>
   </si>
   <si>
-    <t>Master Blaster (Jammin)</t>
-  </si>
-  <si>
-    <t>Dont Stand So Close To Me</t>
+    <t>Master Blaster (Jammin')</t>
+  </si>
+  <si>
+    <t>Don't Stand So Close To Me</t>
   </si>
   <si>
     <t>Wish You Were Here</t>
   </si>
   <si>
-    <t>Dont Stop Believin</t>
+    <t>Don't Stop Believin'</t>
   </si>
   <si>
     <t>The Day Before You Came</t>
@@ -3034,10 +3034,10 @@
     <t>Everytime I Think of You - 2000 Remaster</t>
   </si>
   <si>
-    <t>Dont You Want Me</t>
-  </si>
-  <si>
-    <t>Ill Find My Way Home - Remastered</t>
+    <t>Don't You Want Me</t>
+  </si>
+  <si>
+    <t>I'll Find My Way Home - Remastered</t>
   </si>
   <si>
     <t>Je Loog Tegen Mij</t>
@@ -3118,13 +3118,13 @@
     <t>P.Y.T. (Pretty Young Thing)</t>
   </si>
   <si>
-    <t>Wanna Be Startin Somethin</t>
-  </si>
-  <si>
-    <t>Its Raining Again</t>
-  </si>
-  <si>
-    <t>Steppin Out</t>
+    <t>Wanna Be Startin' Somethin'</t>
+  </si>
+  <si>
+    <t>It's Raining Again</t>
+  </si>
+  <si>
+    <t>Steppin' Out</t>
   </si>
   <si>
     <t>A Slow Song</t>
@@ -3145,10 +3145,10 @@
     <t>Sweet Dreams (Are Made of This) - Remastered</t>
   </si>
   <si>
-    <t>Im Still Standing</t>
-  </si>
-  <si>
-    <t>Lets Dance - 2018 Remaster</t>
+    <t>I'm Still Standing</t>
+  </si>
+  <si>
+    <t>Let's Dance - 2018 Remaster</t>
   </si>
   <si>
     <t>China Girl - 2002 Remaster</t>
@@ -3160,7 +3160,7 @@
     <t>Waterfront - 2002 Remaster</t>
   </si>
   <si>
-    <t>Just Cant Get Enough (Live in Hammersmith) - 2018 Remaster</t>
+    <t>Just Can't Get Enough (Live in Hammersmith) - 2018 Remaster</t>
   </si>
   <si>
     <t>Message To My Girl</t>
@@ -3211,7 +3211,7 @@
     <t>When The Lady Smiles</t>
   </si>
   <si>
-    <t>Summer Of 69</t>
+    <t>Summer Of '69</t>
   </si>
   <si>
     <t>Radio Ga Ga - 2011 Mix</t>
@@ -3223,7 +3223,7 @@
     <t>Bad - Remastered 2009</t>
   </si>
   <si>
-    <t>Im On Fire</t>
+    <t>I'm On Fire</t>
   </si>
   <si>
     <t>Pride (In The Name Of Love) - Remastered 2009</t>
@@ -3277,7 +3277,7 @@
     <t>Glory Days</t>
   </si>
   <si>
-    <t>Its My Life - 1997 Remaster</t>
+    <t>It's My Life - 1997 Remaster</t>
   </si>
   <si>
     <t>Heaven</t>
@@ -3289,16 +3289,16 @@
     <t>I Would Die 4 U</t>
   </si>
   <si>
-    <t>Thank God Its Christmas - 2011 Remaster</t>
-  </si>
-  <si>
-    <t>Lets Go Crazy</t>
+    <t>Thank God It's Christmas - 2011 Remaster</t>
+  </si>
+  <si>
+    <t>Let's Go Crazy</t>
   </si>
   <si>
     <t>Wake Me up Before You Go-Go</t>
   </si>
   <si>
-    <t>Youll Never Walk Alone</t>
+    <t>You'll Never Walk Alone</t>
   </si>
   <si>
     <t>Run To You</t>
@@ -3307,7 +3307,7 @@
     <t>Perhaps Love</t>
   </si>
   <si>
-    <t>Dont Answer Me</t>
+    <t>Don't Answer Me</t>
   </si>
   <si>
     <t>Nightporter</t>
@@ -3424,13 +3424,13 @@
     <t>Angel Of Death</t>
   </si>
   <si>
-    <t>Livin On A Prayer</t>
+    <t>Livin' On A Prayer</t>
   </si>
   <si>
     <t>Graceland</t>
   </si>
   <si>
-    <t>Dont Give Up - 2012 Remaster</t>
+    <t>Don't Give Up - 2012 Remaster</t>
   </si>
   <si>
     <t>Sometimes It Snows in April</t>
@@ -3448,13 +3448,13 @@
     <t>You Can Call Me Al</t>
   </si>
   <si>
-    <t>Dont Dream Its Over</t>
+    <t>Don't Dream It's Over</t>
   </si>
   <si>
     <t>Land of Confusion - 2007 Remaster</t>
   </si>
   <si>
-    <t>Lifes What You Make It - 1997 Remaster</t>
+    <t>Life's What You Make It - 1997 Remaster</t>
   </si>
   <si>
     <t>There Is a Light That Never Goes Out - 2011 Remaster</t>
@@ -3505,7 +3505,7 @@
     <t>Sledgehammer - 2012 Remaster</t>
   </si>
   <si>
-    <t>Dont Leave Me This Way (with Sarah Jane Morris)</t>
+    <t>Don't Leave Me This Way (with Sarah Jane Morris)</t>
   </si>
   <si>
     <t>The Way It Is</t>
@@ -3514,10 +3514,10 @@
     <t>Walk This Way (feat. Aerosmith)</t>
   </si>
   <si>
-    <t>Ill Be Over You</t>
-  </si>
-  <si>
-    <t>Why Cant This Be Love</t>
+    <t>I'll Be Over You</t>
+  </si>
+  <si>
+    <t>Why Can't This Be Love</t>
   </si>
   <si>
     <t>In Your Eyes - 2012 Remaster</t>
@@ -3538,7 +3538,7 @@
     <t>Invisible Touch - 2007 Remaster</t>
   </si>
   <si>
-    <t>Sweet Child O Mine</t>
+    <t>Sweet Child O' Mine</t>
   </si>
   <si>
     <t>With Or Without You - Remastered</t>
@@ -3547,7 +3547,7 @@
     <t>Where The Streets Have No Name - Remastered</t>
   </si>
   <si>
-    <t>I Still Havent Found What Im Looking For</t>
+    <t>I Still Haven't Found What I'm Looking For</t>
   </si>
   <si>
     <t>Paradise City</t>
@@ -3577,7 +3577,7 @@
     <t>Alone</t>
   </si>
   <si>
-    <t>Sign O the Times</t>
+    <t>Sign 'O' the Times</t>
   </si>
   <si>
     <t>Never Tear Us Apart</t>
@@ -3634,7 +3634,7 @@
     <t>Brilliant Disguise</t>
   </si>
   <si>
-    <t>Its a Sin - 2001 Remaster</t>
+    <t>It's a Sin - 2001 Remaster</t>
   </si>
   <si>
     <t>Bullet The Blue Sky</t>
@@ -3643,7 +3643,7 @@
     <t>Wonderful Life</t>
   </si>
   <si>
-    <t>Its The End Of The World As We Know It (And I Feel Fine)</t>
+    <t>It's The End Of The World As We Know It (And I Feel Fine)</t>
   </si>
   <si>
     <t>Is This Love - 2018 Remaster</t>
@@ -3739,7 +3739,7 @@
     <t>Sympathy For The Devil</t>
   </si>
   <si>
-    <t>Rockin in the Free World</t>
+    <t>Rockin' in the Free World</t>
   </si>
   <si>
     <t>Poison</t>
@@ -3778,10 +3778,10 @@
     <t>Woman In Chains</t>
   </si>
   <si>
-    <t>If You Dont Know Me by Now - 2008 Remaster</t>
-  </si>
-  <si>
-    <t>Free Fallin</t>
+    <t>If You Don't Know Me by Now - 2008 Remaster</t>
+  </si>
+  <si>
+    <t>Free Fallin'</t>
   </si>
   <si>
     <t>Epic</t>
@@ -3790,7 +3790,7 @@
     <t>Black Velvet</t>
   </si>
   <si>
-    <t>We Didnt Start the Fire</t>
+    <t>We Didn't Start the Fire</t>
   </si>
   <si>
     <t>Sowing The Seeds Of Love</t>
@@ -3847,7 +3847,7 @@
     <t>Send Me An Angel</t>
   </si>
   <si>
-    <t>Dont Go Breaking My Heart</t>
+    <t>Don't Go Breaking My Heart</t>
   </si>
   <si>
     <t>Night Fever - From Saturday Night Fever Soundtrack</t>
@@ -3913,7 +3913,7 @@
     <t>Jeremy</t>
   </si>
   <si>
-    <t>Knockin On Heavens Door</t>
+    <t>Knockin' On Heaven's Door</t>
   </si>
   <si>
     <t>The Unforgiven</t>
@@ -3940,7 +3940,7 @@
     <t>Year of the Cat - 2001 Remaster</t>
   </si>
   <si>
-    <t>Dont Cry (Original)</t>
+    <t>Don't Cry (Original)</t>
   </si>
   <si>
     <t>(Everything I Do) I Do It For You</t>
@@ -3985,7 +3985,7 @@
     <t>Stars</t>
   </si>
   <si>
-    <t>Im Going Slightly Mad - Remastered 2011</t>
+    <t>I'm Going Slightly Mad - Remastered 2011</t>
   </si>
   <si>
     <t>On the Border - 2001 Remaster</t>
@@ -3994,13 +3994,13 @@
     <t>Diamonds and Pearls</t>
   </si>
   <si>
-    <t>I Cant Dance - 2007 Remaster</t>
+    <t>I Can't Dance - 2007 Remaster</t>
   </si>
   <si>
     <t>No Son of Mine - 2007 Remaster</t>
   </si>
   <si>
-    <t>I Cant Make You Love Me</t>
+    <t>I Can't Make You Love Me</t>
   </si>
   <si>
     <t>Love of the Common People</t>
@@ -4009,7 +4009,7 @@
     <t>Mysterious Ways</t>
   </si>
   <si>
-    <t>We Dont Need Another Hero (Thunderdome)</t>
+    <t>We Don't Need Another Hero (Thunderdome)</t>
   </si>
   <si>
     <t>Calling Elvis</t>
@@ -4042,7 +4042,7 @@
     <t>Would?</t>
   </si>
   <si>
-    <t>Friday Im in Love</t>
+    <t>Friday I'm in Love</t>
   </si>
   <si>
     <t>Sharp Dressed Man</t>
@@ -4051,10 +4051,10 @@
     <t>Man On The Moon</t>
   </si>
   <si>
-    <t>Gimme All Your Lovin</t>
-  </si>
-  <si>
-    <t>Whats Up?</t>
+    <t>Gimme All Your Lovin'</t>
+  </si>
+  <si>
+    <t>What's Up?</t>
   </si>
   <si>
     <t>Lavender</t>
@@ -4075,7 +4075,7 @@
     <t>Remedy</t>
   </si>
   <si>
-    <t>Ive Got Dreams to Remember</t>
+    <t>I've Got Dreams to Remember</t>
   </si>
   <si>
     <t>Jump Around</t>
@@ -4123,7 +4123,7 @@
     <t>Alles Geprobeerd</t>
   </si>
   <si>
-    <t>Id Do Anything For Love (But I Wont Do That) - Single Edit</t>
+    <t>I'd Do Anything For Love (But I Won't Do That) - Single Edit</t>
   </si>
   <si>
     <t>I Will Survive - Single Version</t>
@@ -4156,7 +4156,7 @@
     <t>Cose della vita</t>
   </si>
   <si>
-    <t>Whats Love Got to Do with It</t>
+    <t>What's Love Got to Do with It</t>
   </si>
   <si>
     <t>Rearviewmirror (Remastered)</t>
@@ -4243,7 +4243,7 @@
     <t>Wonderwall - Remastered</t>
   </si>
   <si>
-    <t>Dont Look Back In Anger - Remastered</t>
+    <t>Don't Look Back In Anger - Remastered</t>
   </si>
   <si>
     <t>Streets of Philadelphia - Single Edit</t>
@@ -4270,7 +4270,7 @@
     <t>Circle Of Life</t>
   </si>
   <si>
-    <t>They Dont Care About Us</t>
+    <t>They Don't Care About Us</t>
   </si>
   <si>
     <t>Champagne Supernova - Remastered</t>
@@ -4285,13 +4285,13 @@
     <t>Weak</t>
   </si>
   <si>
-    <t>Gangstas Paradise</t>
+    <t>Gangsta's Paradise</t>
   </si>
   <si>
     <t>Con Te Partirò</t>
   </si>
   <si>
-    <t>Dont Speak</t>
+    <t>Don't Speak</t>
   </si>
   <si>
     <t>Heaven For Everyone - Remastered 2011</t>
@@ -4309,7 +4309,7 @@
     <t>Avalon</t>
   </si>
   <si>
-    <t>You Dont Fool Me - Remastered 2011</t>
+    <t>You Don't Fool Me - Remastered 2011</t>
   </si>
   <si>
     <t>Can You Feel The Love Tonight</t>
@@ -4336,7 +4336,7 @@
     <t>Bullet With Butterfly Wings - Remastered 2012</t>
   </si>
   <si>
-    <t>A Winters Tale - 2011 Remaster</t>
+    <t>A Winter's Tale - 2011 Remaster</t>
   </si>
   <si>
     <t>High And Dry</t>
@@ -4384,7 +4384,7 @@
     <t>Beautiful Goodbye</t>
   </si>
   <si>
-    <t>Aint Nobody</t>
+    <t>Ain't Nobody</t>
   </si>
   <si>
     <t>A Long December</t>
@@ -4444,25 +4444,25 @@
     <t>My Heart Will Go On - Love Theme from Titanic</t>
   </si>
   <si>
-    <t>t Dondert En t Bliksemt</t>
+    <t>t Dondert En 't Bliksemt</t>
   </si>
   <si>
     <t>The Memory Remains</t>
   </si>
   <si>
-    <t>Noubliez Jamais</t>
+    <t>N'oubliez Jamais</t>
   </si>
   <si>
     <t>Tell Him</t>
   </si>
   <si>
-    <t>Cant Stand Losing You</t>
+    <t>Can't Stand Losing You</t>
   </si>
   <si>
     <t>Songbird</t>
   </si>
   <si>
-    <t>The Drugs Dont Work</t>
+    <t>The Drugs Don't Work</t>
   </si>
   <si>
     <t>Around the World</t>
@@ -4474,7 +4474,7 @@
     <t>Careless Whisper</t>
   </si>
   <si>
-    <t>Dont Let the Sun Go Down on Me</t>
+    <t>Don't Let the Sun Go Down on Me</t>
   </si>
   <si>
     <t>The Whole of the Moon</t>
@@ -4486,7 +4486,7 @@
     <t>Narcotic - Long Version</t>
   </si>
   <si>
-    <t>New Years Day</t>
+    <t>New Year's Day</t>
   </si>
   <si>
     <t>Cowboys and Angels</t>
@@ -4498,7 +4498,7 @@
     <t>Toen Ik Je Zag - Single Version</t>
   </si>
   <si>
-    <t>I Dont Want to Miss a Thing - From Armageddon Soundtrack</t>
+    <t>I Don't Want to Miss a Thing - From Armageddon Soundtrack</t>
   </si>
   <si>
     <t>Fields Of Gold</t>
@@ -4516,10 +4516,10 @@
     <t>Freak On a Leash</t>
   </si>
   <si>
-    <t>Non non rien na changé</t>
-  </si>
-  <si>
-    <t>Killer / Papa Was a Rollin Stone</t>
+    <t>Non non rien n'a changé</t>
+  </si>
+  <si>
+    <t>Killer / Papa Was a Rollin' Stone</t>
   </si>
   <si>
     <t>I Knew You Were Waiting (For Me)</t>
@@ -4543,7 +4543,7 @@
     <t>Pure Morning</t>
   </si>
   <si>
-    <t>Shes The One</t>
+    <t>She's The One</t>
   </si>
   <si>
     <t>Pretty Fly (For A White Guy)</t>
@@ -4585,7 +4585,7 @@
     <t>Let Me Entertain You</t>
   </si>
   <si>
-    <t>Road Trippin</t>
+    <t>Road Trippin'</t>
   </si>
   <si>
     <t>Jesus He Knows Me</t>
@@ -4600,7 +4600,7 @@
     <t>LA Song</t>
   </si>
   <si>
-    <t>The Dolphins Cry</t>
+    <t>The Dolphin's Cry</t>
   </si>
   <si>
     <t>All Star</t>
@@ -4633,7 +4633,7 @@
     <t>At Last</t>
   </si>
   <si>
-    <t>Cant Help Falling in Love</t>
+    <t>Can't Help Falling in Love</t>
   </si>
   <si>
     <t>Fly Me To The Moon (In Other Words)</t>
@@ -4648,7 +4648,7 @@
     <t>Ring of Fire</t>
   </si>
   <si>
-    <t>Blowin in the Wind</t>
+    <t>Blowin' in the Wind</t>
   </si>
   <si>
     <t>In Dreams</t>
@@ -4657,7 +4657,7 @@
     <t>Are You Lonesome Tonight</t>
   </si>
   <si>
-    <t>Dont Think Twice, Its All Right</t>
+    <t>Don't Think Twice, It's All Right</t>
   </si>
   <si>
     <t>The Sound of Silence - Acoustic Version</t>
@@ -4669,16 +4669,16 @@
     <t>Folsom Prison Blues</t>
   </si>
   <si>
-    <t>The Times They Are A-Changin</t>
+    <t>The Times They Are A-Changin'</t>
   </si>
   <si>
     <t>A Change Is Gonna Come</t>
   </si>
   <si>
-    <t>Its All Over Now - Mono Version</t>
-  </si>
-  <si>
-    <t>(I Cant Get No) Satisfaction - Mono Version</t>
+    <t>It's All Over Now - Mono Version</t>
+  </si>
+  <si>
+    <t>(I Can't Get No) Satisfaction - Mono Version</t>
   </si>
   <si>
     <t>Like a Rolling Stone</t>
@@ -4711,16 +4711,16 @@
     <t>God Only Knows - Remastered</t>
   </si>
   <si>
-    <t>California Dreamin - Single Version</t>
+    <t>California Dreamin' - Single Version</t>
   </si>
   <si>
     <t>River Deep - Mountain High</t>
   </si>
   <si>
-    <t>Thats Life</t>
-  </si>
-  <si>
-    <t>Jumpin Jack Flash - Mono</t>
+    <t>That's Life</t>
+  </si>
+  <si>
+    <t>Jumpin' Jack Flash - Mono</t>
   </si>
   <si>
     <t>Scarborough Fair / Canticle</t>
@@ -4747,13 +4747,13 @@
     <t>Monday, Monday - Single Version</t>
   </si>
   <si>
-    <t>Its A Mans, Mans, Mans World</t>
+    <t>It's A Man's, Man's, Man's World</t>
   </si>
   <si>
     <t>Try a Little Tenderness</t>
   </si>
   <si>
-    <t>Wouldnt It Be Nice - Stereo Mix</t>
+    <t>Wouldn't It Be Nice - Stereo Mix</t>
   </si>
   <si>
     <t>Nights In White Satin - Single Version / Mono Mix</t>
@@ -4798,19 +4798,19 @@
     <t>Ruby Tuesday</t>
   </si>
   <si>
-    <t>He Aint Heavy, Hes My Brother</t>
+    <t>He Ain't Heavy, He's My Brother</t>
   </si>
   <si>
     <t>Guitar Man</t>
   </si>
   <si>
-    <t>Aint No Mountain High Enough</t>
+    <t>Ain't No Mountain High Enough</t>
   </si>
   <si>
     <t>San Francisco (Be Sure to Wear Some Flowers In Your Hair)</t>
   </si>
   <si>
-    <t>Im a Believer - 2006 Remaster</t>
+    <t>I'm a Believer - 2006 Remaster</t>
   </si>
   <si>
     <t>Waterloo Sunset - Mono Mix</t>
@@ -4831,7 +4831,7 @@
     <t>Pastorale - Remastered</t>
   </si>
   <si>
-    <t>(Sittin On) the Dock of the Bay</t>
+    <t>(Sittin' On) the Dock of the Bay</t>
   </si>
   <si>
     <t>I Put A Spell On You</t>
@@ -4861,7 +4861,7 @@
     <t>The Weight - Remastered</t>
   </si>
   <si>
-    <t>Aint Got No - I Got Life - Remastered</t>
+    <t>Ain't Got No - I Got Life - Remastered</t>
   </si>
   <si>
     <t>Voodoo Child (Slight Return)</t>
@@ -4888,13 +4888,13 @@
     <t>MacArthur Park</t>
   </si>
   <si>
-    <t>Id Rather Go Blind</t>
+    <t>I'd Rather Go Blind</t>
   </si>
   <si>
     <t>Daydream Believer</t>
   </si>
   <si>
-    <t>Girl, Youll Be A Woman Soon</t>
+    <t>Girl, You'll Be A Woman Soon</t>
   </si>
   <si>
     <t>Space Oddity - 2015 Remaster</t>
@@ -4921,7 +4921,7 @@
     <t>Bad Moon Rising</t>
   </si>
   <si>
-    <t>You Cant Always Get What You Want</t>
+    <t>You Can't Always Get What You Want</t>
   </si>
   <si>
     <t>With A Little Help From My Friends</t>
@@ -5083,7 +5083,7 @@
     <t>Herbert Grönemeyer</t>
   </si>
   <si>
-    <t>Youssou NDour</t>
+    <t>Youssou N'Dour</t>
   </si>
   <si>
     <t>Robert Plant</t>
@@ -5290,7 +5290,7 @@
     <t>Neil Young</t>
   </si>
   <si>
-    <t>De Poemas</t>
+    <t>De Poema's</t>
   </si>
   <si>
     <t>Nightwish</t>
@@ -5404,7 +5404,7 @@
     <t>Wolfmother</t>
   </si>
   <si>
-    <t>Ks Choice</t>
+    <t>K's Choice</t>
   </si>
   <si>
     <t>Kim Wilde</t>
@@ -5626,7 +5626,7 @@
     <t>DJ Paul</t>
   </si>
   <si>
-    <t>Sniff n The Tears</t>
+    <t>Sniff 'n' The Tears</t>
   </si>
   <si>
     <t>Foster The People</t>
@@ -5752,7 +5752,7 @@
     <t>Dotan</t>
   </si>
   <si>
-    <t>Gigi DAgostino</t>
+    <t>Gigi D'Agostino</t>
   </si>
   <si>
     <t>The Who</t>
@@ -5845,7 +5845,7 @@
     <t>The Trammps</t>
   </si>
   <si>
-    <t>Q65</t>
+    <t>Q'65</t>
   </si>
   <si>
     <t>Lukas Graham</t>
@@ -5854,7 +5854,7 @@
     <t>Jason Paige</t>
   </si>
   <si>
-    <t>RagnBone Man</t>
+    <t>Rag'n'Bone Man</t>
   </si>
   <si>
     <t>Harry Styles</t>
@@ -6043,7 +6043,7 @@
     <t>The Cats</t>
   </si>
   <si>
-    <t>Gilbert OSullivan</t>
+    <t>Gilbert O'Sullivan</t>
   </si>
   <si>
     <t>Carole King</t>
@@ -6211,7 +6211,7 @@
     <t>Ramones</t>
   </si>
   <si>
-    <t>Manfred Manns Earth Band</t>
+    <t>Manfred Mann's Earth Band</t>
   </si>
   <si>
     <t>Diana Ross</t>
@@ -6493,10 +6493,10 @@
     <t>Pet Shop Boys</t>
   </si>
   <si>
-    <t>Guns N Roses</t>
-  </si>
-  <si>
-    <t>Sinéad OConnor</t>
+    <t>Guns N' Roses</t>
+  </si>
+  <si>
+    <t>Sinéad O'Connor</t>
   </si>
   <si>
     <t>Whitesnake</t>
@@ -6565,7 +6565,7 @@
     <t>Cher</t>
   </si>
   <si>
-    <t>The B-52s</t>
+    <t>The B-52's</t>
   </si>
   <si>
     <t>Queensrÿche</t>

</xml_diff>